<commit_message>
Now reads data from mongodb
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhaarun\Desktop\lead\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhaarun\Desktop\kriya-lead\kriya-leaderboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AA05BD-7119-4A81-A01C-98FCBCF11C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13265056-0B65-4D87-86E5-2DD415FACAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13332" yWindow="3360" windowWidth="9708" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14244" yWindow="1308" windowWidth="9708" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,7 +366,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +423,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>